<commit_message>
changed upload ages order
</commit_message>
<xml_diff>
--- a/template_spreadsheet.xlsx
+++ b/template_spreadsheet.xlsx
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="196">
   <si>
     <t>Column</t>
   </si>
@@ -560,7 +560,7 @@
     <t>Total.210Pb.Alpha..synonym.Total.210Po.</t>
   </si>
   <si>
-    <t>210Pb/210Po</t>
+    <t>210Pb alpha</t>
   </si>
   <si>
     <t>Total.210Pb.Alpha..synonym.Total.210Po..Units</t>
@@ -575,7 +575,7 @@
     <t>Total.210Pb.Gamma</t>
   </si>
   <si>
-    <t>210Pb</t>
+    <t>210Pb gamma</t>
   </si>
   <si>
     <t>Total.210Pb.Gamma.Units</t>
@@ -632,6 +632,9 @@
     <t>Supported.210Pb</t>
   </si>
   <si>
+    <t>Supported 210Pb</t>
+  </si>
+  <si>
     <t>Supported.210Pb.Units</t>
   </si>
   <si>
@@ -686,6 +689,12 @@
     <t>The format is the regex for a DOI</t>
   </si>
   <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>ndb.publications.publicationid</t>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
@@ -714,12 +723,6 @@
   </si>
   <si>
     <t>ndb.leadmodels.cumulativeinventory</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>ndb.contactreferences.contactid</t>
   </si>
 </sst>
 </file>
@@ -2220,12 +2223,8 @@
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="21" style="18" customWidth="1"/>
-    <col min="2" max="2" width="28" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.67188" style="18" customWidth="1"/>
-    <col min="4" max="4" width="10.1719" style="18" customWidth="1"/>
-    <col min="5" max="5" width="9.17188" style="18" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="18" customWidth="1"/>
-    <col min="7" max="13" width="24.8516" style="18" customWidth="1"/>
+    <col min="2" max="10" width="11.5" style="18" customWidth="1"/>
+    <col min="11" max="13" width="24.8516" style="18" customWidth="1"/>
     <col min="14" max="14" width="24.5" style="18" customWidth="1"/>
     <col min="15" max="16" width="31.5" style="18" customWidth="1"/>
     <col min="17" max="16384" width="11.5" style="18" customWidth="1"/>
@@ -4317,7 +4316,7 @@
       </c>
       <c r="N67" s="21"/>
       <c r="O67" s="21"/>
-      <c r="P67" s="21"/>
+      <c r="P67" s="20"/>
     </row>
     <row r="68" ht="13.65" customHeight="1">
       <c r="A68" t="s" s="19">
@@ -4355,7 +4354,7 @@
       </c>
       <c r="N68" s="21"/>
       <c r="O68" s="21"/>
-      <c r="P68" s="21"/>
+      <c r="P68" s="20"/>
     </row>
     <row r="69" ht="13.65" customHeight="1">
       <c r="A69" t="s" s="19">
@@ -4397,7 +4396,9 @@
       <c r="O69" t="s" s="20">
         <v>144</v>
       </c>
-      <c r="P69" s="21"/>
+      <c r="P69" t="s" s="20">
+        <v>105</v>
+      </c>
     </row>
     <row r="70" ht="13.65" customHeight="1">
       <c r="A70" t="s" s="19">
@@ -4439,7 +4440,9 @@
       <c r="O70" t="s" s="20">
         <v>149</v>
       </c>
-      <c r="P70" s="21"/>
+      <c r="P70" t="s" s="20">
+        <v>105</v>
+      </c>
     </row>
     <row r="71" ht="13.65" customHeight="1">
       <c r="A71" t="s" s="19">
@@ -4481,7 +4484,9 @@
       <c r="O71" t="s" s="20">
         <v>154</v>
       </c>
-      <c r="P71" s="21"/>
+      <c r="P71" t="s" s="20">
+        <v>105</v>
+      </c>
     </row>
     <row r="72" ht="13.65" customHeight="1">
       <c r="A72" t="s" s="19">
@@ -4523,7 +4528,9 @@
       <c r="O72" t="s" s="20">
         <v>159</v>
       </c>
-      <c r="P72" s="21"/>
+      <c r="P72" t="s" s="20">
+        <v>105</v>
+      </c>
     </row>
     <row r="73" ht="13.65" customHeight="1">
       <c r="A73" t="s" s="19">
@@ -4565,7 +4572,9 @@
       <c r="O73" t="s" s="20">
         <v>163</v>
       </c>
-      <c r="P73" s="21"/>
+      <c r="P73" t="s" s="20">
+        <v>105</v>
+      </c>
     </row>
     <row r="74" ht="13.65" customHeight="1">
       <c r="A74" t="s" s="19">
@@ -4591,19 +4600,19 @@
       <c r="I74" s="8"/>
       <c r="J74" s="21"/>
       <c r="K74" t="s" s="24">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="L74" t="s" s="20">
         <v>138</v>
       </c>
       <c r="M74" t="s" s="20">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N74" t="s" s="20">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O74" t="s" s="20">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="P74" t="s" s="20">
         <v>105</v>
@@ -4611,7 +4620,7 @@
     </row>
     <row r="75" ht="13.65" customHeight="1">
       <c r="A75" t="s" s="19">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B75" t="s" s="5">
         <v>132</v>
@@ -4633,19 +4642,19 @@
       <c r="I75" s="8"/>
       <c r="J75" s="21"/>
       <c r="K75" t="s" s="24">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L75" t="s" s="20">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M75" t="s" s="20">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N75" t="s" s="20">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O75" t="s" s="20">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="P75" t="s" s="20">
         <v>105</v>
@@ -4653,7 +4662,7 @@
     </row>
     <row r="76" ht="13.65" customHeight="1">
       <c r="A76" t="s" s="19">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B76" t="s" s="5">
         <v>132</v>
@@ -4675,28 +4684,30 @@
       <c r="I76" s="8"/>
       <c r="J76" s="21"/>
       <c r="K76" t="s" s="24">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L76" t="s" s="20">
         <v>138</v>
       </c>
       <c r="M76" t="s" s="20">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N76" t="s" s="20">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O76" t="s" s="20">
-        <v>178</v>
-      </c>
-      <c r="P76" s="21"/>
+        <v>179</v>
+      </c>
+      <c r="P76" t="s" s="20">
+        <v>105</v>
+      </c>
     </row>
     <row r="77" ht="13.65" customHeight="1">
       <c r="A77" t="s" s="19">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B77" t="s" s="5">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C77" t="b" s="6">
         <v>0</v>
@@ -4711,13 +4722,13 @@
         <v>29</v>
       </c>
       <c r="G77" t="s" s="20">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H77" t="s" s="20">
         <v>115</v>
       </c>
       <c r="I77" t="s" s="7">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J77" s="21"/>
       <c r="K77" s="21"/>
@@ -4729,10 +4740,10 @@
     </row>
     <row r="78" ht="13.65" customHeight="1">
       <c r="A78" t="s" s="19">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B78" t="s" s="5">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C78" t="b" s="6">
         <v>0</v>
@@ -4741,15 +4752,13 @@
         <v>0</v>
       </c>
       <c r="E78" t="b" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="s" s="20">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G78" s="21"/>
-      <c r="H78" t="s" s="20">
-        <v>115</v>
-      </c>
+      <c r="H78" s="21"/>
       <c r="I78" s="8"/>
       <c r="J78" s="21"/>
       <c r="K78" s="21"/>
@@ -4761,10 +4770,10 @@
     </row>
     <row r="79" ht="13.65" customHeight="1">
       <c r="A79" t="s" s="19">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B79" t="s" s="5">
-        <v>52</v>
+        <v>187</v>
       </c>
       <c r="C79" t="b" s="6">
         <v>0</v>
@@ -4793,10 +4802,10 @@
     </row>
     <row r="80" ht="13.65" customHeight="1">
       <c r="A80" t="s" s="19">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B80" t="s" s="5">
-        <v>187</v>
+        <v>52</v>
       </c>
       <c r="C80" t="b" s="6">
         <v>0</v>
@@ -4812,7 +4821,7 @@
       </c>
       <c r="G80" s="21"/>
       <c r="H80" t="s" s="20">
-        <v>188</v>
+        <v>115</v>
       </c>
       <c r="I80" s="8"/>
       <c r="J80" s="21"/>
@@ -4840,10 +4849,12 @@
         <v>0</v>
       </c>
       <c r="F81" t="s" s="20">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G81" s="21"/>
-      <c r="H81" s="21"/>
+      <c r="H81" t="s" s="20">
+        <v>191</v>
+      </c>
       <c r="I81" s="8"/>
       <c r="J81" s="21"/>
       <c r="K81" s="21"/>
@@ -4855,10 +4866,10 @@
     </row>
     <row r="82" ht="13.65" customHeight="1">
       <c r="A82" t="s" s="19">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B82" t="s" s="5">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C82" t="b" s="6">
         <v>0</v>
@@ -4885,10 +4896,10 @@
     </row>
     <row r="83" ht="13.65" customHeight="1">
       <c r="A83" t="s" s="19">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B83" t="s" s="5">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C83" t="b" s="6">
         <v>0</v>
@@ -4897,10 +4908,10 @@
         <v>0</v>
       </c>
       <c r="E83" t="b" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" t="s" s="20">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G83" s="21"/>
       <c r="H83" s="21"/>

</xml_diff>